<commit_message>
Estrucutura de nuevas carpetas MVC
</commit_message>
<xml_diff>
--- a/control/Path_Control/autenticacionApi/articulos/data/Productos.xlsx
+++ b/control/Path_Control/autenticacionApi/articulos/data/Productos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
     <t>MLM2127158007</t>
   </si>
   <si>
-    <t>MLM131441</t>
-  </si>
-  <si>
     <t>Llanta Bicicleta Ruta 20x1 1/8 (28-451) R20 P728 Benotto</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>MLM3339189642</t>
-  </si>
-  <si>
-    <t>MLM456634</t>
   </si>
   <si>
     <t>Llanta Delantera Patin Xiam - Producto Prueba No Ofertar</t>
@@ -498,11 +492,8 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2">
         <v>5000</v>
@@ -517,24 +508,21 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="D3">
         <v>547</v>
@@ -546,16 +534,16 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="1">
         <v>0.87</v>
       </c>
       <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>